<commit_message>
Final EDIT Ready to print
</commit_message>
<xml_diff>
--- a/Data_List_Corrected_4.xlsx
+++ b/Data_List_Corrected_4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOWNLOAD\DOWNLOAD_2018\certificates\Faculty and Administrative Staff certificate Design 21April2018_v6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOWNLOAD\DOWNLOAD_2018\certificates\certificate_design_prateek\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="255">
   <si>
     <t xml:space="preserve"> Priyanshi Pal</t>
   </si>
@@ -735,6 +735,60 @@
   </si>
   <si>
     <t>Dr. J N Gangwar</t>
+  </si>
+  <si>
+    <t>Saraush Verma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archit </t>
+  </si>
+  <si>
+    <t>Dr. Y. K. Prajapati</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Priyanshi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soham </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prasoon </t>
+  </si>
+  <si>
+    <t>Karnika</t>
+  </si>
+  <si>
+    <t>Ananya Singh</t>
+  </si>
+  <si>
+    <t>Dr.  N K Singh</t>
+  </si>
+  <si>
+    <t>Ojasvani</t>
+  </si>
+  <si>
+    <t>Aparna</t>
+  </si>
+  <si>
+    <t>Aradhaya</t>
+  </si>
+  <si>
+    <t>Sanvi</t>
+  </si>
+  <si>
+    <t>Dr. Sameer Srivastava</t>
+  </si>
+  <si>
+    <t>Janvi Gangwar</t>
+  </si>
+  <si>
+    <t>Dr. J. N. Gangwar</t>
+  </si>
+  <si>
+    <t>Dr. P. R. Pal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premenshi </t>
   </si>
 </sst>
 </file>
@@ -744,7 +798,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +902,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -884,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -920,9 +1002,6 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -933,9 +1012,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -944,6 +1020,21 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,2253 +1373,2660 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="30"/>
-    <col min="8" max="8" width="10.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="20" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="28"/>
+    <col min="8" max="8" width="10.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="18"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="21">
         <v>42742</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F2" s="23">
+      <c r="E2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="22">
         <v>13</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="23">
         <v>42742</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>42742</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F3" s="23">
+      <c r="E3" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="22">
         <v>14</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>42742</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F4" s="23">
+      <c r="E4" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="22">
         <v>13</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>42742</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="E5" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5" s="22">
         <v>13</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>42742</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F6" s="23">
+      <c r="E6" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" s="22">
         <v>14</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>42742</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="E7" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7" s="22">
         <v>14</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="21">
         <v>42742</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F8" s="23">
+      <c r="E8" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F8" s="22">
         <v>10</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>42742</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F9" s="23">
+      <c r="E9" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F9" s="22">
         <v>10</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <v>42742</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="E10" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F10" s="22">
         <v>8</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="21">
         <v>42742</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F11" s="23">
+      <c r="E11" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="22">
         <v>13</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <v>42742</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="E12" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12" s="22">
         <v>7</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <v>42742</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F13" s="23">
+      <c r="E13" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F13" s="22">
         <v>14</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>42742</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F14" s="23">
+      <c r="E14" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" s="22">
         <v>13</v>
       </c>
-      <c r="G14" s="24"/>
+      <c r="G14" s="29"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <v>42742</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F15" s="23">
+      <c r="E15" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" s="22">
         <v>11</v>
       </c>
-      <c r="G15" s="24"/>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <v>42742</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F16" s="23">
+      <c r="E16" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F16" s="22">
         <v>12</v>
       </c>
-      <c r="G16" s="24"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>42742</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F17" s="23">
+      <c r="E17" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" s="22">
         <v>10</v>
       </c>
-      <c r="G17" s="24"/>
+      <c r="G17" s="29"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>42742</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F18" s="23">
+      <c r="E18" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F18" s="22">
         <v>9</v>
       </c>
-      <c r="G18" s="24"/>
+      <c r="G18" s="29"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="21">
         <v>42742</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F19" s="23">
+      <c r="E19" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F19" s="22">
         <v>8</v>
       </c>
-      <c r="G19" s="24"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>42742</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F20" s="23">
+      <c r="E20" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F20" s="22">
         <v>10</v>
       </c>
-      <c r="G20" s="24"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="21">
         <v>42742</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F21" s="23">
+      <c r="E21" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F21" s="22">
         <v>9</v>
       </c>
-      <c r="G21" s="24"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="21">
         <v>42742</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F22" s="23">
+      <c r="E22" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F22" s="22">
         <v>7</v>
       </c>
-      <c r="G22" s="24"/>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="21">
         <v>42742</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F23" s="23">
+      <c r="E23" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F23" s="22">
         <v>8</v>
       </c>
-      <c r="G23" s="24"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="21">
         <v>42742</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="22">
         <v>14</v>
       </c>
-      <c r="G24" s="24"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="21">
         <v>42742</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="22">
         <v>12</v>
       </c>
-      <c r="G25" s="24"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="21">
         <v>42742</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="22">
         <v>8</v>
       </c>
-      <c r="G26" s="24"/>
+      <c r="G26" s="29"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="21">
         <v>42742</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="22">
         <v>8</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="29"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="27">
         <v>43099</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24" t="s">
+      <c r="F28" s="22"/>
+      <c r="G28" s="29" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="27">
         <v>43099</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="24"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="29"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="27">
         <v>43099</v>
       </c>
-      <c r="E30" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
+      <c r="E30" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F30" s="22"/>
+      <c r="G30" s="29"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="27">
         <v>43099</v>
       </c>
-      <c r="E31" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="24"/>
+      <c r="E31" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="29"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="27">
         <v>43099</v>
       </c>
-      <c r="E32" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="24"/>
+      <c r="E32" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="29"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="27">
         <v>43099</v>
       </c>
-      <c r="E33" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F33" s="23"/>
-      <c r="G33" s="24"/>
+      <c r="E33" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="29"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="27">
         <v>43099</v>
       </c>
-      <c r="E34" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
+      <c r="E34" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F34" s="22"/>
+      <c r="G34" s="29"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="27">
         <v>43099</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="24"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="29"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="27">
         <v>43099</v>
       </c>
-      <c r="E36" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F36" s="23"/>
-      <c r="G36" s="24"/>
+      <c r="E36" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F36" s="22"/>
+      <c r="G36" s="29"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37" s="27">
         <v>43099</v>
       </c>
-      <c r="E37" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F37" s="23"/>
-      <c r="G37" s="24"/>
+      <c r="E37" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" s="22"/>
+      <c r="G37" s="29"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="27">
         <v>43099</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="24"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="29"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="27">
         <v>43099</v>
       </c>
-      <c r="E39" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F39" s="23"/>
-      <c r="G39" s="24"/>
+      <c r="E39" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F39" s="22"/>
+      <c r="G39" s="29"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="27">
         <v>43099</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F40" s="23"/>
-      <c r="G40" s="24"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="29"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="27">
         <v>43099</v>
       </c>
-      <c r="E41" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="24"/>
+      <c r="E41" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F41" s="22"/>
+      <c r="G41" s="29"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="27">
         <v>43099</v>
       </c>
-      <c r="E42" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F42" s="23"/>
-      <c r="G42" s="24"/>
+      <c r="E42" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F42" s="22"/>
+      <c r="G42" s="29"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="27">
         <v>43099</v>
       </c>
-      <c r="E43" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F43" s="23"/>
-      <c r="G43" s="24"/>
+      <c r="E43" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F43" s="22"/>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="27">
         <v>43099</v>
       </c>
-      <c r="E44" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F44" s="23"/>
-      <c r="G44" s="24"/>
+      <c r="E44" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F44" s="22"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45" s="27">
         <v>43099</v>
       </c>
-      <c r="E45" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F45" s="23"/>
-      <c r="G45" s="24"/>
+      <c r="E45" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F45" s="22"/>
+      <c r="G45" s="29"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D46" s="29">
+      <c r="D46" s="27">
         <v>43099</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="E46" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F46" s="23"/>
-      <c r="G46" s="24"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="29"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="27">
         <v>43099</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F47" s="23"/>
-      <c r="G47" s="24"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="29"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D48" s="29">
+      <c r="D48" s="27">
         <v>43099</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F48" s="23"/>
-      <c r="G48" s="24"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="29"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D49" s="29">
+      <c r="D49" s="27">
         <v>43099</v>
       </c>
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F49" s="23"/>
-      <c r="G49" s="24"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="29"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D50" s="29">
+      <c r="D50" s="27">
         <v>43099</v>
       </c>
-      <c r="E50" s="23" t="s">
+      <c r="E50" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F50" s="23"/>
-      <c r="G50" s="24"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="29"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D51" s="29">
+      <c r="D51" s="27">
         <v>43099</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F51" s="23"/>
-      <c r="G51" s="24"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="29"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C52" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D52" s="29">
+      <c r="D52" s="27">
         <v>43099</v>
       </c>
-      <c r="E52" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F52" s="23"/>
-      <c r="G52" s="24"/>
+      <c r="E52" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F52" s="22"/>
+      <c r="G52" s="29"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="23" t="s">
+      <c r="A53" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D53" s="29">
+      <c r="D53" s="27">
         <v>43099</v>
       </c>
-      <c r="E53" s="23" t="s">
+      <c r="E53" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F53" s="23"/>
-      <c r="G53" s="24"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="29"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D54" s="29">
+      <c r="D54" s="27">
         <v>43099</v>
       </c>
-      <c r="E54" s="23" t="s">
+      <c r="E54" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F54" s="23"/>
-      <c r="G54" s="24"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="29"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D55" s="29">
+      <c r="D55" s="27">
         <v>43099</v>
       </c>
-      <c r="E55" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F55" s="23"/>
-      <c r="G55" s="24"/>
+      <c r="E55" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F55" s="22"/>
+      <c r="G55" s="29"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D56" s="29">
+      <c r="D56" s="27">
         <v>43099</v>
       </c>
-      <c r="E56" s="23" t="s">
+      <c r="E56" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F56" s="23"/>
-      <c r="G56" s="24"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="29"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D57" s="29">
+      <c r="D57" s="27">
         <v>43099</v>
       </c>
-      <c r="E57" s="23" t="s">
+      <c r="E57" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F57" s="23"/>
-      <c r="G57" s="24"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="29"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D58" s="29">
+      <c r="D58" s="27">
         <v>43095</v>
       </c>
-      <c r="E58" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F58" s="23"/>
-      <c r="G58" s="24" t="s">
+      <c r="E58" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F58" s="22"/>
+      <c r="G58" s="29" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D59" s="29">
+      <c r="D59" s="27">
         <v>43095</v>
       </c>
-      <c r="E59" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F59" s="23"/>
-      <c r="G59" s="24"/>
+      <c r="E59" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F59" s="22"/>
+      <c r="G59" s="29"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D60" s="29">
+      <c r="D60" s="27">
         <v>43095</v>
       </c>
-      <c r="E60" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F60" s="23"/>
-      <c r="G60" s="24"/>
+      <c r="E60" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F60" s="22"/>
+      <c r="G60" s="29"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="27" t="s">
+      <c r="B61" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D61" s="29">
+      <c r="D61" s="27">
         <v>43095</v>
       </c>
-      <c r="E61" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F61" s="23"/>
-      <c r="G61" s="24"/>
+      <c r="E61" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F61" s="22"/>
+      <c r="G61" s="29"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B62" s="27" t="s">
+      <c r="B62" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C62" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D62" s="29">
+      <c r="D62" s="27">
         <v>43095</v>
       </c>
-      <c r="E62" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F62" s="23"/>
-      <c r="G62" s="24"/>
+      <c r="E62" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F62" s="22"/>
+      <c r="G62" s="29"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="B63" s="27" t="s">
+      <c r="B63" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C63" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D63" s="29">
+      <c r="D63" s="27">
         <v>43095</v>
       </c>
-      <c r="E63" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F63" s="23"/>
-      <c r="G63" s="24"/>
+      <c r="E63" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F63" s="22"/>
+      <c r="G63" s="29"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D64" s="29">
+      <c r="D64" s="27">
         <v>43095</v>
       </c>
-      <c r="E64" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F64" s="23"/>
-      <c r="G64" s="24"/>
+      <c r="E64" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F64" s="22"/>
+      <c r="G64" s="29"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C65" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D65" s="29">
+      <c r="D65" s="27">
         <v>43095</v>
       </c>
-      <c r="E65" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F65" s="23"/>
-      <c r="G65" s="24"/>
+      <c r="E65" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F65" s="22"/>
+      <c r="G65" s="29"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="23" t="s">
+      <c r="A66" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="21" t="s">
+      <c r="B66" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="C66" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D66" s="29">
+      <c r="D66" s="27">
         <v>43095</v>
       </c>
-      <c r="E66" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F66" s="23"/>
-      <c r="G66" s="24"/>
+      <c r="E66" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F66" s="22"/>
+      <c r="G66" s="29"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
+      <c r="A67" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B67" s="21" t="s">
+      <c r="B67" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C67" s="21" t="s">
+      <c r="C67" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D67" s="29">
+      <c r="D67" s="27">
         <v>43095</v>
       </c>
-      <c r="E67" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F67" s="23"/>
-      <c r="G67" s="24"/>
+      <c r="E67" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F67" s="22"/>
+      <c r="G67" s="29"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="21" t="s">
+      <c r="B68" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="21" t="s">
+      <c r="C68" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D68" s="29">
+      <c r="D68" s="27">
         <v>43095</v>
       </c>
-      <c r="E68" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F68" s="23"/>
-      <c r="G68" s="24"/>
+      <c r="E68" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F68" s="22"/>
+      <c r="G68" s="29"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C69" s="21" t="s">
+      <c r="C69" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D69" s="29">
+      <c r="D69" s="27">
         <v>43095</v>
       </c>
-      <c r="E69" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F69" s="23"/>
-      <c r="G69" s="24"/>
+      <c r="E69" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F69" s="22"/>
+      <c r="G69" s="29"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C70" s="21" t="s">
+      <c r="C70" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D70" s="29">
+      <c r="D70" s="27">
         <v>43095</v>
       </c>
-      <c r="E70" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F70" s="23"/>
-      <c r="G70" s="24"/>
+      <c r="E70" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F70" s="22"/>
+      <c r="G70" s="29"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
+      <c r="A71" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C71" s="21" t="s">
+      <c r="C71" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D71" s="29">
+      <c r="D71" s="27">
         <v>43095</v>
       </c>
-      <c r="E71" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F71" s="23"/>
-      <c r="G71" s="24"/>
+      <c r="E71" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F71" s="22"/>
+      <c r="G71" s="29"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="23" t="s">
+      <c r="A72" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D72" s="29">
+      <c r="D72" s="27">
         <v>43095</v>
       </c>
-      <c r="E72" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F72" s="23"/>
-      <c r="G72" s="24"/>
+      <c r="E72" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F72" s="22"/>
+      <c r="G72" s="29"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B73" s="27" t="s">
+      <c r="B73" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="29">
+      <c r="D73" s="27">
         <v>43095</v>
       </c>
-      <c r="E73" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F73" s="23"/>
-      <c r="G73" s="24"/>
+      <c r="E73" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F73" s="22"/>
+      <c r="G73" s="29"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B74" s="27" t="s">
+      <c r="B74" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="C74" s="21" t="s">
+      <c r="C74" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D74" s="29">
+      <c r="D74" s="27">
         <v>43095</v>
       </c>
-      <c r="E74" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F74" s="23"/>
-      <c r="G74" s="24"/>
+      <c r="E74" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F74" s="22"/>
+      <c r="G74" s="29"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="C75" s="21" t="s">
+      <c r="C75" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D75" s="29">
+      <c r="D75" s="27">
         <v>43095</v>
       </c>
-      <c r="E75" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F75" s="23"/>
-      <c r="G75" s="24"/>
+      <c r="E75" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F75" s="22"/>
+      <c r="G75" s="29"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B76" s="21" t="s">
+      <c r="B76" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D76" s="29">
+      <c r="D76" s="27">
         <v>43095</v>
       </c>
-      <c r="E76" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F76" s="23"/>
-      <c r="G76" s="24"/>
+      <c r="E76" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F76" s="22"/>
+      <c r="G76" s="29"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="23" t="s">
+      <c r="A77" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C77" s="21" t="s">
+      <c r="C77" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D77" s="29">
+      <c r="D77" s="27">
         <v>43095</v>
       </c>
-      <c r="E77" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F77" s="23"/>
-      <c r="G77" s="24"/>
+      <c r="E77" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F77" s="22"/>
+      <c r="G77" s="29"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="20" t="s">
+      <c r="A78" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B78" s="21" t="s">
+      <c r="B78" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C78" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D78" s="29">
+      <c r="C78" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D78" s="27">
         <v>43037</v>
       </c>
-      <c r="E78" s="23" t="s">
+      <c r="E78" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F78" s="23"/>
-      <c r="G78" s="24" t="s">
+      <c r="F78" s="22"/>
+      <c r="G78" s="29" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="20" t="s">
+      <c r="A79" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="21" t="s">
+      <c r="B79" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="C79" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D79" s="29">
+      <c r="C79" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D79" s="27">
         <v>43037</v>
       </c>
-      <c r="E79" s="23" t="s">
+      <c r="E79" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F79" s="23"/>
-      <c r="G79" s="24"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="29"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="20" t="s">
+      <c r="A80" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="21" t="s">
+      <c r="B80" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C80" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D80" s="29">
+      <c r="C80" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D80" s="27">
         <v>43037</v>
       </c>
-      <c r="E80" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F80" s="23"/>
-      <c r="G80" s="24"/>
+      <c r="E80" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F80" s="22"/>
+      <c r="G80" s="29"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="20" t="s">
+      <c r="A81" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B81" s="21" t="s">
+      <c r="B81" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C81" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D81" s="29">
+      <c r="C81" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D81" s="27">
         <v>43037</v>
       </c>
-      <c r="E81" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F81" s="23"/>
-      <c r="G81" s="24"/>
+      <c r="E81" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F81" s="22"/>
+      <c r="G81" s="29"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B82" s="21" t="s">
+      <c r="B82" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C82" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D82" s="29">
+      <c r="C82" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D82" s="27">
         <v>43037</v>
       </c>
-      <c r="E82" s="23" t="s">
+      <c r="E82" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F82" s="23"/>
-      <c r="G82" s="24"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="29"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="20" t="s">
+      <c r="A83" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="21" t="s">
+      <c r="B83" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C83" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D83" s="29">
+      <c r="C83" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D83" s="27">
         <v>43037</v>
       </c>
-      <c r="E83" s="23" t="s">
+      <c r="E83" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F83" s="23"/>
-      <c r="G83" s="24"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="29"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="21" t="s">
+      <c r="B84" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="C84" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D84" s="29">
+      <c r="C84" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D84" s="27">
         <v>43037</v>
       </c>
-      <c r="E84" s="23" t="s">
+      <c r="E84" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F84" s="23"/>
-      <c r="G84" s="24"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="29"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C85" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D85" s="29">
+      <c r="C85" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D85" s="27">
         <v>43037</v>
       </c>
-      <c r="E85" s="23" t="s">
+      <c r="E85" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F85" s="23"/>
-      <c r="G85" s="24"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="29"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="20" t="s">
+      <c r="A86" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B86" s="21" t="s">
+      <c r="B86" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C86" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D86" s="29">
+      <c r="C86" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D86" s="27">
         <v>43037</v>
       </c>
-      <c r="E86" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F86" s="23"/>
-      <c r="G86" s="24"/>
+      <c r="E86" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F86" s="22"/>
+      <c r="G86" s="29"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C87" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D87" s="29">
+      <c r="C87" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D87" s="27">
         <v>43037</v>
       </c>
-      <c r="E87" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F87" s="23"/>
-      <c r="G87" s="24"/>
+      <c r="E87" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F87" s="22"/>
+      <c r="G87" s="29"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="20" t="s">
+      <c r="A88" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B88" s="21" t="s">
+      <c r="B88" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C88" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D88" s="29">
+      <c r="C88" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D88" s="27">
         <v>43037</v>
       </c>
-      <c r="E88" s="23" t="s">
+      <c r="E88" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F88" s="23"/>
-      <c r="G88" s="24"/>
+      <c r="F88" s="22"/>
+      <c r="G88" s="29"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="20" t="s">
+      <c r="A89" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B89" s="21" t="s">
+      <c r="B89" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="C89" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D89" s="29">
+      <c r="C89" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D89" s="27">
         <v>43037</v>
       </c>
-      <c r="E89" s="23" t="s">
+      <c r="E89" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F89" s="23"/>
-      <c r="G89" s="24"/>
+      <c r="F89" s="22"/>
+      <c r="G89" s="29"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="20" t="s">
+      <c r="A90" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B90" s="21" t="s">
+      <c r="B90" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C90" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D90" s="29">
+      <c r="C90" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D90" s="27">
         <v>43037</v>
       </c>
-      <c r="E90" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F90" s="23"/>
-      <c r="G90" s="24"/>
+      <c r="E90" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F90" s="22"/>
+      <c r="G90" s="29"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="28" t="s">
+      <c r="A91" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B91" s="27" t="s">
+      <c r="B91" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="C91" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D91" s="29">
+      <c r="C91" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D91" s="27">
         <v>43037</v>
       </c>
-      <c r="E91" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F91" s="23"/>
-      <c r="G91" s="24"/>
+      <c r="E91" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F91" s="22"/>
+      <c r="G91" s="29"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="20" t="s">
+      <c r="A92" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="23" t="s">
+      <c r="B92" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C92" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D92" s="29">
+      <c r="C92" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D92" s="27">
         <v>43037</v>
       </c>
-      <c r="E92" s="23" t="s">
+      <c r="E92" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F92" s="23"/>
-      <c r="G92" s="24"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="29"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="20" t="s">
+      <c r="A93" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B93" s="21" t="s">
+      <c r="B93" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C93" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D93" s="29">
+      <c r="C93" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D93" s="27">
         <v>43037</v>
       </c>
-      <c r="E93" s="23" t="s">
+      <c r="E93" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F93" s="23"/>
-      <c r="G93" s="24"/>
+      <c r="F93" s="22"/>
+      <c r="G93" s="29"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="20" t="s">
+      <c r="A94" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B94" s="21" t="s">
+      <c r="B94" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C94" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D94" s="29">
+      <c r="C94" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D94" s="27">
         <v>43037</v>
       </c>
-      <c r="E94" s="23" t="s">
+      <c r="E94" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F94" s="23"/>
-      <c r="G94" s="24"/>
+      <c r="F94" s="22"/>
+      <c r="G94" s="29"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="28" t="s">
+      <c r="A95" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B95" s="21" t="s">
+      <c r="B95" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C95" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D95" s="29">
+      <c r="C95" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D95" s="27">
         <v>43037</v>
       </c>
-      <c r="E95" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F95" s="23"/>
-      <c r="G95" s="24"/>
+      <c r="E95" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F95" s="22"/>
+      <c r="G95" s="29"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="s">
+      <c r="A96" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="B96" s="21" t="s">
+      <c r="B96" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C96" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D96" s="29">
+      <c r="C96" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D96" s="27">
         <v>43037</v>
       </c>
-      <c r="E96" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F96" s="23"/>
-      <c r="G96" s="24"/>
+      <c r="E96" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F96" s="22"/>
+      <c r="G96" s="29"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="20" t="s">
+      <c r="A97" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B97" s="21" t="s">
+      <c r="B97" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C97" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D97" s="29">
+      <c r="C97" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D97" s="27">
         <v>43037</v>
       </c>
-      <c r="E97" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F97" s="23"/>
-      <c r="G97" s="24"/>
+      <c r="E97" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F97" s="22"/>
+      <c r="G97" s="29"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="20" t="s">
+      <c r="A98" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B98" s="21" t="s">
+      <c r="B98" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C98" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D98" s="29">
+      <c r="C98" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D98" s="27">
         <v>43037</v>
       </c>
-      <c r="E98" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F98" s="23"/>
-      <c r="G98" s="24"/>
+      <c r="E98" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F98" s="22"/>
+      <c r="G98" s="29"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="20" t="s">
+      <c r="A99" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C99" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D99" s="29">
+      <c r="C99" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D99" s="27">
         <v>43037</v>
       </c>
-      <c r="E99" s="23" t="s">
+      <c r="E99" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F99" s="23"/>
-      <c r="G99" s="24"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="29"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="20" t="s">
+      <c r="A100" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B100" s="21" t="s">
+      <c r="B100" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C100" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D100" s="29">
+      <c r="C100" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D100" s="27">
         <v>43037</v>
       </c>
-      <c r="E100" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F100" s="23"/>
-      <c r="G100" s="24"/>
+      <c r="E100" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F100" s="22"/>
+      <c r="G100" s="29"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="21" t="s">
+      <c r="B101" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C101" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D101" s="29">
+      <c r="C101" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D101" s="27">
         <v>43037</v>
       </c>
-      <c r="E101" s="23" t="s">
+      <c r="E101" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F101" s="23"/>
-      <c r="G101" s="24"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="29"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="20" t="s">
+      <c r="A102" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B102" s="23" t="s">
+      <c r="B102" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C102" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D102" s="29">
+      <c r="C102" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D102" s="27">
         <v>43037</v>
       </c>
-      <c r="E102" s="23" t="s">
+      <c r="E102" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F102" s="23"/>
-      <c r="G102" s="24"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="29"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="20" t="s">
+      <c r="A103" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B103" s="21" t="s">
+      <c r="B103" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C103" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D103" s="29">
+      <c r="C103" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D103" s="27">
         <v>43037</v>
       </c>
-      <c r="E103" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F103" s="23"/>
-      <c r="G103" s="24"/>
+      <c r="E103" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F103" s="22"/>
+      <c r="G103" s="29"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="20" t="s">
+      <c r="A104" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B104" s="21" t="s">
+      <c r="B104" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C104" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D104" s="29">
+      <c r="C104" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D104" s="27">
         <v>43037</v>
       </c>
-      <c r="E104" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F104" s="23"/>
-      <c r="G104" s="24"/>
+      <c r="E104" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F104" s="22"/>
+      <c r="G104" s="29"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="20" t="s">
+      <c r="A105" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B105" s="21" t="s">
+      <c r="B105" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C105" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D105" s="29">
+      <c r="C105" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D105" s="27">
         <v>43037</v>
       </c>
-      <c r="E105" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F105" s="23"/>
-      <c r="G105" s="24"/>
+      <c r="E105" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F105" s="22"/>
+      <c r="G105" s="29"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="20" t="s">
+      <c r="A106" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B106" s="21" t="s">
+      <c r="B106" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C106" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D106" s="29">
+      <c r="C106" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D106" s="27">
         <v>43037</v>
       </c>
-      <c r="E106" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F106" s="23"/>
-      <c r="G106" s="24"/>
+      <c r="E106" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F106" s="22"/>
+      <c r="G106" s="29"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="20" t="s">
+      <c r="A107" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B107" s="21" t="s">
+      <c r="B107" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C107" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D107" s="29">
+      <c r="C107" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D107" s="27">
         <v>43037</v>
       </c>
-      <c r="E107" s="23" t="s">
+      <c r="E107" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F107" s="23"/>
-      <c r="G107" s="24"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="29"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="20" t="s">
+      <c r="A108" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B108" s="21" t="s">
+      <c r="B108" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C108" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D108" s="29">
+      <c r="C108" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D108" s="27">
         <v>43037</v>
       </c>
-      <c r="E108" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F108" s="23"/>
-      <c r="G108" s="24"/>
+      <c r="E108" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F108" s="22"/>
+      <c r="G108" s="29"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="20" t="s">
+      <c r="A109" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C109" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D109" s="29">
+      <c r="C109" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D109" s="27">
         <v>43037</v>
       </c>
-      <c r="E109" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F109" s="23"/>
-      <c r="G109" s="24"/>
+      <c r="E109" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F109" s="22"/>
+      <c r="G109" s="29"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="20" t="s">
+      <c r="A110" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="21" t="s">
+      <c r="B110" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C110" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D110" s="29">
+      <c r="C110" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D110" s="27">
         <v>43037</v>
       </c>
-      <c r="E110" s="23" t="s">
+      <c r="E110" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F110" s="23"/>
-      <c r="G110" s="24"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="29"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="20" t="s">
+      <c r="A111" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B111" s="21" t="s">
+      <c r="B111" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C111" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D111" s="29">
+      <c r="C111" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D111" s="27">
         <v>43037</v>
       </c>
-      <c r="E111" s="23" t="s">
+      <c r="E111" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F111" s="23"/>
-      <c r="G111" s="24"/>
+      <c r="F111" s="22"/>
+      <c r="G111" s="29"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="20" t="s">
+      <c r="A112" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B112" s="21" t="s">
+      <c r="B112" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C112" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D112" s="29">
+      <c r="C112" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D112" s="27">
         <v>43037</v>
       </c>
-      <c r="E112" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F112" s="23"/>
-      <c r="G112" s="24"/>
+      <c r="E112" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F112" s="22"/>
+      <c r="G112" s="29"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="20" t="s">
+      <c r="A113" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B113" s="21" t="s">
+      <c r="B113" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C113" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D113" s="29">
+      <c r="C113" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D113" s="27">
         <v>43037</v>
       </c>
-      <c r="E113" s="23" t="s">
+      <c r="E113" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F113" s="23"/>
-      <c r="G113" s="24"/>
+      <c r="F113" s="22"/>
+      <c r="G113" s="29"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="20" t="s">
+      <c r="A114" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B114" s="21" t="s">
+      <c r="B114" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C114" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D114" s="29">
+      <c r="C114" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D114" s="27">
         <v>43037</v>
       </c>
-      <c r="E114" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F114" s="23"/>
-      <c r="G114" s="24"/>
+      <c r="E114" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F114" s="22"/>
+      <c r="G114" s="29"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B115" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="C115" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D115" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E115" s="33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="B116" s="35"/>
+      <c r="C116" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D116" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E116" s="33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D117" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E117" s="33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" s="35"/>
+      <c r="C118" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D118" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E118" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B119" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C119" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D119" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E119" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B120" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C120" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D120" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E120" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B121" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="C121" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D121" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E121" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="B122" s="31"/>
+      <c r="C122" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D122" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E122" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B123" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="C123" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D123" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E123" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B124" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C124" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D124" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E124" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B125" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C125" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D125" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E125" s="36" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="B126" s="35"/>
+      <c r="C126" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D126" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E126" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B127" s="35"/>
+      <c r="C127" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D127" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E127" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B128" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C128" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D128" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E128" s="36" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B129" s="35"/>
+      <c r="C129" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D129" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E129" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="B130" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="C130" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D130" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E130" s="36" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="B131" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C131" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D131" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E131" s="36" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="B132" s="35"/>
+      <c r="C132" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D132" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E132" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="B133" s="35"/>
+      <c r="C133" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D133" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E133" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="B134" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C134" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D134" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E134" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="B135" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="C135" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D135" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E135" s="37" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="C136" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D136" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E136" s="37" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B137" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C137" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D137" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E137" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="B138" s="35"/>
+      <c r="C138" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D138" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E138" s="39" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B139" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C139" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D139" s="32">
+        <v>43126</v>
+      </c>
+      <c r="E139" s="31" t="s">
+        <v>211</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5174,7 +5672,7 @@
       <c r="G2" s="3">
         <v>4</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="30" t="s">
         <v>90</v>
       </c>
       <c r="I2" s="3">
@@ -5203,7 +5701,7 @@
       <c r="G3" s="3">
         <v>4</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="30"/>
       <c r="I3" s="3">
         <v>3</v>
       </c>
@@ -5231,7 +5729,7 @@
       <c r="G4" s="3">
         <v>4</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="30"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="39" x14ac:dyDescent="0.25">
@@ -5254,7 +5752,7 @@
       <c r="G5" s="3">
         <v>4</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="39" x14ac:dyDescent="0.25">
@@ -5279,7 +5777,7 @@
       <c r="G6" s="3">
         <v>5</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="3">
         <v>1</v>
       </c>
@@ -5306,7 +5804,7 @@
       <c r="G7" s="3">
         <v>5</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="3">
         <v>2</v>
       </c>
@@ -5333,7 +5831,7 @@
       <c r="G8" s="3">
         <v>5</v>
       </c>
-      <c r="H8" s="15"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="3">
         <v>2</v>
       </c>
@@ -5360,7 +5858,7 @@
       <c r="G9" s="3">
         <v>5</v>
       </c>
-      <c r="H9" s="15"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="3">
         <v>3</v>
       </c>
@@ -5385,7 +5883,7 @@
       <c r="G10" s="3">
         <v>6</v>
       </c>
-      <c r="H10" s="15"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:15" ht="39" x14ac:dyDescent="0.25">
@@ -5408,7 +5906,7 @@
       <c r="G11" s="3">
         <v>7</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="30" t="s">
         <v>91</v>
       </c>
       <c r="I11" s="3"/>
@@ -5435,7 +5933,7 @@
       <c r="G12" s="3">
         <v>7</v>
       </c>
-      <c r="H12" s="15"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="3">
         <v>2</v>
       </c>
@@ -5462,7 +5960,7 @@
       <c r="G13" s="3">
         <v>7</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="3">
         <v>3</v>
       </c>
@@ -5487,7 +5985,7 @@
       <c r="G14" s="3">
         <v>7</v>
       </c>
-      <c r="H14" s="15"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:15" ht="39" x14ac:dyDescent="0.25">
@@ -5510,7 +6008,7 @@
       <c r="G15" s="3">
         <v>7</v>
       </c>
-      <c r="H15" s="15"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="39" x14ac:dyDescent="0.25">
@@ -5535,7 +6033,7 @@
       <c r="G16" s="3">
         <v>8</v>
       </c>
-      <c r="H16" s="15"/>
+      <c r="H16" s="30"/>
       <c r="I16" s="3">
         <v>1</v>
       </c>
@@ -5562,7 +6060,7 @@
       <c r="G17" s="3">
         <v>8</v>
       </c>
-      <c r="H17" s="15"/>
+      <c r="H17" s="30"/>
       <c r="I17" s="3">
         <v>1</v>
       </c>
@@ -5589,7 +6087,7 @@
       <c r="G18" s="3">
         <v>8</v>
       </c>
-      <c r="H18" s="15"/>
+      <c r="H18" s="30"/>
       <c r="I18" s="3">
         <v>3</v>
       </c>
@@ -5614,7 +6112,7 @@
       <c r="G19" s="3">
         <v>8</v>
       </c>
-      <c r="H19" s="15"/>
+      <c r="H19" s="30"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5637,7 +6135,7 @@
       <c r="G20" s="3">
         <v>8</v>
       </c>
-      <c r="H20" s="15"/>
+      <c r="H20" s="30"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5660,7 +6158,7 @@
       <c r="G21" s="3">
         <v>8</v>
       </c>
-      <c r="H21" s="15"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5683,7 +6181,7 @@
       <c r="G22" s="3">
         <v>8</v>
       </c>
-      <c r="H22" s="15"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5708,7 +6206,7 @@
       <c r="G23" s="3">
         <v>9</v>
       </c>
-      <c r="H23" s="15"/>
+      <c r="H23" s="30"/>
       <c r="I23" s="3">
         <v>2</v>
       </c>
@@ -5733,7 +6231,7 @@
       <c r="G24" s="3">
         <v>9</v>
       </c>
-      <c r="H24" s="15"/>
+      <c r="H24" s="30"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5758,7 +6256,7 @@
       <c r="G25" s="3">
         <v>10</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="30" t="s">
         <v>92</v>
       </c>
       <c r="I25" s="3">
@@ -5787,7 +6285,7 @@
       <c r="G26" s="3">
         <v>10</v>
       </c>
-      <c r="H26" s="15"/>
+      <c r="H26" s="30"/>
       <c r="I26" s="3">
         <v>3</v>
       </c>
@@ -5812,7 +6310,7 @@
       <c r="G27" s="3">
         <v>10</v>
       </c>
-      <c r="H27" s="15"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5835,7 +6333,7 @@
       <c r="G28" s="3">
         <v>10</v>
       </c>
-      <c r="H28" s="15"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5858,7 +6356,7 @@
       <c r="G29" s="3">
         <v>10</v>
       </c>
-      <c r="H29" s="15"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5881,7 +6379,7 @@
       <c r="G30" s="3">
         <v>10</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5906,7 +6404,7 @@
       <c r="G31" s="3">
         <v>11</v>
       </c>
-      <c r="H31" s="15"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="3">
         <v>2</v>
       </c>
@@ -5931,7 +6429,7 @@
       <c r="G32" s="3">
         <v>11</v>
       </c>
-      <c r="H32" s="15"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5954,7 +6452,7 @@
       <c r="G33" s="3">
         <v>11</v>
       </c>
-      <c r="H33" s="15"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -5979,7 +6477,7 @@
       <c r="G34" s="3">
         <v>12</v>
       </c>
-      <c r="H34" s="15"/>
+      <c r="H34" s="30"/>
       <c r="I34" s="3">
         <v>1</v>
       </c>
@@ -6006,7 +6504,7 @@
       <c r="G35" s="3">
         <v>12</v>
       </c>
-      <c r="H35" s="15"/>
+      <c r="H35" s="30"/>
       <c r="I35" s="3">
         <v>3</v>
       </c>
@@ -6031,7 +6529,7 @@
       <c r="G36" s="3">
         <v>12</v>
       </c>
-      <c r="H36" s="15"/>
+      <c r="H36" s="30"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -6056,7 +6554,7 @@
       <c r="G37" s="3">
         <v>13</v>
       </c>
-      <c r="H37" s="15"/>
+      <c r="H37" s="30"/>
       <c r="I37" s="3">
         <v>1</v>
       </c>
@@ -6081,7 +6579,7 @@
       <c r="G38" s="3">
         <v>13</v>
       </c>
-      <c r="H38" s="15"/>
+      <c r="H38" s="30"/>
       <c r="I38" s="3"/>
     </row>
   </sheetData>

</xml_diff>